<commit_message>
Modification des premiers fichiers SQL et ajout de TI
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_04_03.xlsx
+++ b/Excel/TI/Mon_TI_2024_04_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL31"/>
+  <dimension ref="A1:AL30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,101 +628,87 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Anthony Davis</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Questionable</t>
-        </is>
-      </c>
+          <t>Kevin Durant</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="G2" t="n">
-        <v>48.1</v>
+        <v>37.7</v>
       </c>
       <c r="H2" t="n">
-        <v>47.9</v>
+        <v>42.6</v>
       </c>
       <c r="I2" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N2" t="n">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="O2" t="n">
+        <v>37</v>
+      </c>
+      <c r="P2" t="n">
+        <v>52</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>50</v>
+      </c>
+      <c r="R2" t="n">
         <v>44</v>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q2" t="n">
-        <v>59</v>
-      </c>
-      <c r="R2" t="n">
-        <v>70</v>
-      </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>-1.2</v>
-      </c>
-      <c r="U2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="V2" t="n">
-        <v>11</v>
-      </c>
+        <v>1.9</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="Z2" t="n">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
@@ -751,7 +737,7 @@
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
@@ -761,7 +747,7 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
@@ -771,7 +757,7 @@
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
@@ -781,66 +767,80 @@
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>LAC</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kevin Durant</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>Kyle Kuzma</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Day-To-Day</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>F</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F3" t="n">
-        <v>41</v>
+        <v>25.2</v>
       </c>
       <c r="G3" t="n">
-        <v>37.7</v>
+        <v>34.2</v>
       </c>
       <c r="H3" t="n">
-        <v>42.6</v>
+        <v>29.9</v>
       </c>
       <c r="I3" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J3" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" t="n">
+        <v>4</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
         <v>1</v>
       </c>
-      <c r="K3" t="n">
-        <v>4</v>
-      </c>
-      <c r="L3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" t="n">
-        <v>7</v>
-      </c>
-      <c r="N3" t="n">
-        <v>22</v>
-      </c>
-      <c r="O3" t="n">
-        <v>37</v>
-      </c>
-      <c r="P3" t="n">
-        <v>52</v>
-      </c>
       <c r="Q3" t="n">
-        <v>50</v>
-      </c>
-      <c r="R3" t="n">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -848,10 +848,14 @@
         </is>
       </c>
       <c r="T3" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
+        <v>-0.8</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="V3" t="n">
+        <v>11</v>
+      </c>
       <c r="W3" t="inlineStr">
         <is>
           <t>vs</t>
@@ -859,7 +863,7 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -868,7 +872,7 @@
         </is>
       </c>
       <c r="Z3" t="n">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
@@ -897,49 +901,49 @@
       </c>
       <c r="AF3" t="inlineStr">
         <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>NOP</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>LAC</t>
-        </is>
-      </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>CHI</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cade Cunningham</t>
+          <t>Anthony Edwards</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -948,68 +952,72 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F4" t="n">
-        <v>39.2</v>
+        <v>25.6</v>
       </c>
       <c r="G4" t="n">
-        <v>33.5</v>
+        <v>34.1</v>
       </c>
       <c r="H4" t="n">
-        <v>32.1</v>
+        <v>36.3</v>
       </c>
       <c r="I4" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L4" t="n">
         <v>3</v>
       </c>
       <c r="M4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N4" t="n">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="O4" t="n">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="P4" t="n">
-        <v>38</v>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>32</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>8</v>
+      </c>
+      <c r="R4" t="n">
+        <v>33</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T4" t="n">
-        <v>-1.6</v>
-      </c>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
+        <v>-1.1</v>
+      </c>
+      <c r="U4" t="n">
+        <v>-2.8</v>
+      </c>
+      <c r="V4" t="n">
+        <v>11</v>
+      </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -1018,15 +1026,17 @@
         </is>
       </c>
       <c r="Z4" t="n">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AB4" t="n">
-        <v>14</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
@@ -1045,7 +1055,7 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
@@ -1055,86 +1065,84 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>DEN</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Donovan Mitchell</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
+          <t>Cade Cunningham</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Questionable</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>G</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>16</v>
+        <v>39.2</v>
       </c>
       <c r="G5" t="n">
         <v>33.5</v>
       </c>
       <c r="H5" t="n">
-        <v>37.9</v>
+        <v>32.1</v>
       </c>
       <c r="I5" t="n">
+        <v>12</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
         <v>4</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" t="n">
         <v>4</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
       <c r="N5" t="n">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="O5" t="n">
-        <v>17</v>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>44</v>
+      </c>
+      <c r="P5" t="n">
+        <v>38</v>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
@@ -1152,14 +1160,10 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>-4.3</v>
-      </c>
-      <c r="U5" t="n">
-        <v>-10.9</v>
-      </c>
-      <c r="V5" t="n">
-        <v>6</v>
-      </c>
+        <v>-1.6</v>
+      </c>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr">
         <is>
           <t>@</t>
@@ -1167,28 +1171,24 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="Z5" t="n">
+        <v>72</v>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AB5" t="n">
+        <v>14</v>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
@@ -1217,17 +1217,17 @@
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
@@ -1237,25 +1237,25 @@
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>CHI</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Anthony Edwards</t>
+          <t>Evan Mobley</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1264,75 +1264,77 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>26</v>
+        <v>36.4</v>
       </c>
       <c r="G6" t="n">
-        <v>33.1</v>
+        <v>32.3</v>
       </c>
       <c r="H6" t="n">
-        <v>36.4</v>
+        <v>32.5</v>
       </c>
       <c r="I6" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
         <v>2</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="n">
         <v>3</v>
       </c>
-      <c r="L6" t="n">
-        <v>3</v>
-      </c>
-      <c r="M6" t="n">
-        <v>5</v>
-      </c>
       <c r="N6" t="n">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="O6" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="P6" t="n">
+        <v>43</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>24</v>
+      </c>
+      <c r="R6" t="n">
+        <v>33</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="T6" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="V6" t="n">
         <v>8</v>
       </c>
-      <c r="Q6" t="n">
-        <v>33</v>
-      </c>
-      <c r="R6" t="n">
-        <v>29</v>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="T6" t="n">
-        <v>-0.9</v>
-      </c>
-      <c r="U6" t="n">
-        <v>-2.9</v>
-      </c>
-      <c r="V6" t="n">
-        <v>11</v>
-      </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z6" t="n">
-        <v>35</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
@@ -1361,7 +1363,7 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
@@ -1371,7 +1373,7 @@
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
@@ -1381,17 +1383,17 @@
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>IND</t>
         </is>
       </c>
     </row>
@@ -1546,18 +1548,18 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Evan Mobley</t>
+          <t>RJ Barrett</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1566,22 +1568,22 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>33.4</v>
+        <v>35</v>
       </c>
       <c r="G8" t="n">
-        <v>31.8</v>
+        <v>31.6</v>
       </c>
       <c r="H8" t="n">
-        <v>32.3</v>
+        <v>27.8</v>
       </c>
       <c r="I8" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -1590,19 +1592,27 @@
         <v>2</v>
       </c>
       <c r="N8" t="n">
-        <v>41</v>
-      </c>
-      <c r="O8" t="n">
-        <v>43</v>
-      </c>
-      <c r="P8" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>33</v>
-      </c>
-      <c r="R8" t="n">
-        <v>26</v>
+        <v>46</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
@@ -1610,13 +1620,13 @@
         </is>
       </c>
       <c r="T8" t="n">
-        <v>1.5</v>
+        <v>-0.7</v>
       </c>
       <c r="U8" t="n">
-        <v>0.7</v>
+        <v>-7.8</v>
       </c>
       <c r="V8" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="W8" t="inlineStr">
         <is>
@@ -1625,18 +1635,16 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="Z8" t="n">
+        <v>18</v>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
@@ -1665,17 +1673,17 @@
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
@@ -1685,17 +1693,17 @@
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AK8" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>BKN</t>
         </is>
       </c>
     </row>
@@ -2142,97 +2150,93 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Deni Avdija</t>
+          <t>Jalen Duren</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G12" t="n">
-        <v>30.7</v>
+        <v>29.5</v>
       </c>
       <c r="H12" t="n">
-        <v>25.4</v>
+        <v>31</v>
       </c>
       <c r="I12" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K12" t="n">
         <v>3</v>
       </c>
       <c r="L12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M12" t="n">
+        <v>2</v>
+      </c>
+      <c r="N12" t="n">
         <v>1</v>
       </c>
-      <c r="N12" t="n">
-        <v>30</v>
-      </c>
       <c r="O12" t="n">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="P12" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R12" t="n">
-        <v>35</v>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T12" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="U12" t="n">
-        <v>-3.4</v>
-      </c>
-      <c r="V12" t="n">
-        <v>10</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z12" t="n">
-        <v>37</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
@@ -2256,12 +2260,12 @@
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr">
@@ -2271,7 +2275,7 @@
       </c>
       <c r="AH12" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AI12" t="inlineStr">
@@ -2281,7 +2285,7 @@
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="AK12" t="inlineStr">
@@ -2298,156 +2302,146 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jalen Duren</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Day-To-Day</t>
-        </is>
-      </c>
+          <t>Miles Bridges</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="G13" t="n">
+        <v>28.7</v>
+      </c>
+      <c r="H13" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="I13" t="n">
+        <v>14</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" t="n">
+        <v>6</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2</v>
+      </c>
+      <c r="M13" t="n">
+        <v>4</v>
+      </c>
+      <c r="N13" t="n">
+        <v>41</v>
+      </c>
+      <c r="O13" t="n">
+        <v>49</v>
+      </c>
+      <c r="P13" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q13" t="n">
         <v>24</v>
       </c>
-      <c r="G13" t="n">
-        <v>29.5</v>
-      </c>
-      <c r="H13" t="n">
-        <v>31</v>
-      </c>
-      <c r="I13" t="n">
-        <v>12</v>
-      </c>
-      <c r="J13" t="n">
-        <v>3</v>
-      </c>
-      <c r="K13" t="n">
-        <v>3</v>
-      </c>
-      <c r="L13" t="n">
-        <v>4</v>
-      </c>
-      <c r="M13" t="n">
-        <v>2</v>
-      </c>
-      <c r="N13" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" t="n">
-        <v>50</v>
-      </c>
-      <c r="P13" t="n">
-        <v>27</v>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="R13" t="n">
+        <v>14</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>0.5</v>
+        <v>3.1</v>
       </c>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="Z13" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>OKC</t>
+        </is>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AL13" t="inlineStr">
+        <is>
           <t>ATL</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE13" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AF13" t="inlineStr">
-        <is>
-          <t>MEM</t>
-        </is>
-      </c>
-      <c r="AG13" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AH13" t="inlineStr">
-        <is>
-          <t>BKN</t>
-        </is>
-      </c>
-      <c r="AI13" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AJ13" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
-      <c r="AK13" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AL13" t="inlineStr">
-        <is>
-          <t>CHI</t>
         </is>
       </c>
     </row>
@@ -2474,54 +2468,54 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>33.6</v>
+        <v>27.2</v>
       </c>
       <c r="G14" t="n">
-        <v>29.1</v>
+        <v>28.5</v>
       </c>
       <c r="H14" t="n">
-        <v>25.9</v>
+        <v>25.7</v>
       </c>
       <c r="I14" t="n">
         <v>13</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" t="n">
         <v>7</v>
       </c>
       <c r="L14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
         <v>3</v>
       </c>
       <c r="N14" t="n">
+        <v>13</v>
+      </c>
+      <c r="O14" t="n">
         <v>22</v>
       </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
         <v>25</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>21</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
         <v>55</v>
       </c>
-      <c r="R14" t="n">
-        <v>45</v>
-      </c>
       <c r="S14" t="inlineStr">
         <is>
           <t>@</t>
         </is>
       </c>
       <c r="T14" t="n">
-        <v>-0.7</v>
+        <v>-0.8</v>
       </c>
       <c r="U14" t="n">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="V14" t="n">
         <v>13</v>
@@ -2608,87 +2602,95 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Miles Bridges</t>
+          <t>D'Angelo Russell</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F15" t="n">
-        <v>31.4</v>
+        <v>27</v>
       </c>
       <c r="G15" t="n">
-        <v>28.7</v>
+        <v>28.3</v>
       </c>
       <c r="H15" t="n">
-        <v>30.2</v>
+        <v>26.3</v>
       </c>
       <c r="I15" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J15" t="n">
+        <v>5</v>
+      </c>
+      <c r="K15" t="n">
         <v>2</v>
-      </c>
-      <c r="K15" t="n">
-        <v>6</v>
       </c>
       <c r="L15" t="n">
         <v>2</v>
       </c>
       <c r="M15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N15" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="O15" t="n">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="P15" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q15" t="n">
         <v>29</v>
       </c>
-      <c r="Q15" t="n">
-        <v>24</v>
-      </c>
       <c r="R15" t="n">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T15" t="n">
+        <v>-1.6</v>
+      </c>
+      <c r="U15" t="n">
         <v>3.1</v>
       </c>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
+      <c r="V15" t="n">
+        <v>11</v>
+      </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="Z15" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
@@ -2717,7 +2719,7 @@
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr">
@@ -2727,7 +2729,7 @@
       </c>
       <c r="AH15" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AI15" t="inlineStr">
@@ -2737,7 +2739,7 @@
       </c>
       <c r="AJ15" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="AK15" t="inlineStr">
@@ -2747,66 +2749,72 @@
       </c>
       <c r="AL15" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>MEM</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Bradley Beal</t>
+          <t>Deni Avdija</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F16" t="n">
-        <v>21.6</v>
+        <v>33.4</v>
       </c>
       <c r="G16" t="n">
-        <v>28.1</v>
+        <v>28.3</v>
       </c>
       <c r="H16" t="n">
-        <v>26.3</v>
+        <v>25.6</v>
       </c>
       <c r="I16" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
         <v>3</v>
       </c>
-      <c r="K16" t="n">
-        <v>5</v>
-      </c>
       <c r="L16" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M16" t="n">
         <v>1</v>
       </c>
       <c r="N16" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="O16" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="P16" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="Q16" t="n">
-        <v>16</v>
-      </c>
-      <c r="R16" t="n">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
@@ -2814,10 +2822,14 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>-1</v>
-      </c>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
+        <v>0.3</v>
+      </c>
+      <c r="U16" t="n">
+        <v>-3.6</v>
+      </c>
+      <c r="V16" t="n">
+        <v>10</v>
+      </c>
       <c r="W16" t="inlineStr">
         <is>
           <t>vs</t>
@@ -2825,7 +2837,7 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
@@ -2834,7 +2846,7 @@
         </is>
       </c>
       <c r="Z16" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AA16" t="inlineStr">
         <is>
@@ -2863,55 +2875,55 @@
       </c>
       <c r="AF16" t="inlineStr">
         <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="AI16" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="AG16" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AH16" t="inlineStr">
-        <is>
-          <t>NOP</t>
-        </is>
-      </c>
-      <c r="AI16" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AJ16" t="inlineStr">
-        <is>
-          <t>LAC</t>
-        </is>
-      </c>
       <c r="AK16" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL16" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>CHI</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>D'Angelo Russell</t>
+          <t>Khris Middleton</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -2920,77 +2932,77 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>23.4</v>
+        <v>25.4</v>
       </c>
       <c r="G17" t="n">
-        <v>28.1</v>
+        <v>28.3</v>
       </c>
       <c r="H17" t="n">
-        <v>26.2</v>
+        <v>24.1</v>
       </c>
       <c r="I17" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J17" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
         <v>2</v>
       </c>
       <c r="M17" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N17" t="n">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O17" t="n">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="P17" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="Q17" t="n">
-        <v>47</v>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>17</v>
+      </c>
+      <c r="R17" t="n">
+        <v>23</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T17" t="n">
-        <v>-1.7</v>
+        <v>0.4</v>
       </c>
       <c r="U17" t="n">
-        <v>3.2</v>
+        <v>-1.1</v>
       </c>
       <c r="V17" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z17" t="n">
-        <v>26</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA17" t="inlineStr">
         <is>
@@ -3019,7 +3031,7 @@
       </c>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr">
@@ -3029,7 +3041,7 @@
       </c>
       <c r="AH17" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AI17" t="inlineStr">
@@ -3039,76 +3051,76 @@
       </c>
       <c r="AJ17" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AK17" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL17" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>ORL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Nic Claxton</t>
+          <t>Bradley Beal</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>25.6</v>
+        <v>21.6</v>
       </c>
       <c r="G18" t="n">
-        <v>28</v>
+        <v>28.1</v>
       </c>
       <c r="H18" t="n">
-        <v>27.8</v>
+        <v>26.3</v>
       </c>
       <c r="I18" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K18" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L18" t="n">
         <v>5</v>
       </c>
       <c r="M18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N18" t="n">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="O18" t="n">
         <v>21</v>
       </c>
       <c r="P18" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="Q18" t="n">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="R18" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
@@ -3116,7 +3128,7 @@
         </is>
       </c>
       <c r="T18" t="n">
-        <v>-0.3</v>
+        <v>-1</v>
       </c>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
@@ -3127,7 +3139,7 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
@@ -3136,15 +3148,17 @@
         </is>
       </c>
       <c r="Z18" t="n">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AB18" t="n">
-        <v>24</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC18" t="inlineStr">
         <is>
@@ -3163,7 +3177,7 @@
       </c>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr">
@@ -3173,7 +3187,7 @@
       </c>
       <c r="AH18" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AI18" t="inlineStr">
@@ -3183,7 +3197,7 @@
       </c>
       <c r="AJ18" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AK18" t="inlineStr">
@@ -3193,112 +3207,102 @@
       </c>
       <c r="AL18" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>LAC</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Rui Hachimura</t>
+          <t>Nic Claxton</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>32</v>
+        <v>25.6</v>
       </c>
       <c r="G19" t="n">
-        <v>25.8</v>
+        <v>28</v>
       </c>
       <c r="H19" t="n">
-        <v>19.8</v>
+        <v>27.8</v>
       </c>
       <c r="I19" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J19" t="n">
+        <v>2</v>
+      </c>
+      <c r="K19" t="n">
+        <v>7</v>
+      </c>
+      <c r="L19" t="n">
         <v>4</v>
-      </c>
-      <c r="K19" t="n">
-        <v>4</v>
-      </c>
-      <c r="L19" t="n">
-        <v>3</v>
       </c>
       <c r="M19" t="n">
         <v>2</v>
       </c>
       <c r="N19" t="n">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="O19" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="P19" t="n">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="Q19" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="R19" t="n">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T19" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="U19" t="n">
-        <v>6.6</v>
-      </c>
-      <c r="V19" t="n">
-        <v>11</v>
-      </c>
+        <v>-0.3</v>
+      </c>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="Z19" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AA19" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AB19" t="n">
+        <v>24</v>
       </c>
       <c r="AC19" t="inlineStr">
         <is>
@@ -3317,7 +3321,7 @@
       </c>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr">
@@ -3327,7 +3331,7 @@
       </c>
       <c r="AH19" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="AI19" t="inlineStr">
@@ -3337,7 +3341,7 @@
       </c>
       <c r="AJ19" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AK19" t="inlineStr">
@@ -3347,29 +3351,25 @@
       </c>
       <c r="AL19" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>NYK</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Khris Middleton</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Probable</t>
-        </is>
-      </c>
+          <t>Terry Rozier</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -3378,128 +3378,120 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>26.4</v>
+        <v>31.6</v>
       </c>
       <c r="G20" t="n">
-        <v>25.4</v>
+        <v>27.5</v>
       </c>
       <c r="H20" t="n">
-        <v>23.9</v>
+        <v>28.4</v>
       </c>
       <c r="I20" t="n">
+        <v>15</v>
+      </c>
+      <c r="J20" t="n">
+        <v>4</v>
+      </c>
+      <c r="K20" t="n">
         <v>6</v>
       </c>
-      <c r="J20" t="n">
+      <c r="L20" t="n">
         <v>2</v>
       </c>
-      <c r="K20" t="n">
-        <v>1</v>
-      </c>
-      <c r="L20" t="n">
-        <v>1</v>
-      </c>
       <c r="M20" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N20" t="n">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="O20" t="n">
+        <v>40</v>
+      </c>
+      <c r="P20" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>13</v>
+      </c>
+      <c r="R20" t="n">
+        <v>17</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="T20" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="U20" t="n">
+        <v>-6.8</v>
+      </c>
+      <c r="V20" t="n">
         <v>7</v>
       </c>
-      <c r="P20" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q20" t="n">
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="Z20" t="n">
         <v>23</v>
       </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="T20" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="U20" t="n">
-        <v>-0.9</v>
-      </c>
-      <c r="V20" t="n">
-        <v>1</v>
-      </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="X20" t="inlineStr">
-        <is>
-          <t>MEM</t>
-        </is>
-      </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AB20" t="n">
+        <v>24</v>
       </c>
       <c r="AC20" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AD20" t="n">
+        <v>-1</v>
       </c>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH20" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AI20" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ20" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="AK20" t="inlineStr">
@@ -3509,29 +3501,25 @@
       </c>
       <c r="AL20" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>DAL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Terry Rozier</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Probable</t>
-        </is>
-      </c>
+          <t>Rui Hachimura</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -3540,130 +3528,134 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>23.2</v>
+        <v>34.4</v>
       </c>
       <c r="G21" t="n">
-        <v>25.4</v>
+        <v>26.7</v>
       </c>
       <c r="H21" t="n">
-        <v>27.9</v>
+        <v>19.9</v>
       </c>
       <c r="I21" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J21" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M21" t="n">
         <v>2</v>
       </c>
       <c r="N21" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="O21" t="n">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="P21" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>61</v>
+      </c>
+      <c r="R21" t="n">
+        <v>30</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="T21" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="U21" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="V21" t="n">
+        <v>11</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr">
+        <is>
+          <t>WAS</t>
+        </is>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z21" t="n">
         <v>13</v>
       </c>
-      <c r="Q21" t="n">
-        <v>17</v>
-      </c>
-      <c r="R21" t="n">
-        <v>14</v>
-      </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="T21" t="n">
-        <v>-2.7</v>
-      </c>
-      <c r="U21" t="n">
-        <v>-6.3</v>
-      </c>
-      <c r="V21" t="n">
-        <v>7</v>
-      </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="X21" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z21" t="n">
-        <v>23</v>
-      </c>
       <c r="AA21" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AB21" t="n">
-        <v>24</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC21" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AD21" t="n">
-        <v>-1</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH21" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AI21" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ21" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="AK21" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL21" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>MEM</t>
         </is>
       </c>
     </row>
@@ -3690,10 +3682,10 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>13.6</v>
+        <v>20.4</v>
       </c>
       <c r="G22" t="n">
-        <v>25.3</v>
+        <v>25.7</v>
       </c>
       <c r="H22" t="n">
         <v>30.1</v>
@@ -3705,38 +3697,36 @@
         <v>5</v>
       </c>
       <c r="K22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M22" t="n">
         <v>3</v>
       </c>
       <c r="N22" t="n">
+        <v>34</v>
+      </c>
+      <c r="O22" t="n">
         <v>-2</v>
       </c>
-      <c r="O22" t="n">
+      <c r="P22" t="n">
         <v>38</v>
       </c>
-      <c r="P22" t="n">
+      <c r="Q22" t="n">
         <v>5</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="R22" t="n">
         <v>27</v>
       </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="S22" t="inlineStr">
         <is>
           <t>@</t>
         </is>
       </c>
       <c r="T22" t="n">
-        <v>-0.6</v>
+        <v>-0.5</v>
       </c>
       <c r="U22" t="n">
         <v>-7.4</v>
@@ -3834,7 +3824,11 @@
           <t>Brandon Miller</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Questionable</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>F</t>
@@ -4138,10 +4132,10 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>6</v>
+        <v>8.6</v>
       </c>
       <c r="G25" t="n">
-        <v>9.300000000000001</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H25" t="n">
         <v>16.8</v>
@@ -4162,32 +4156,30 @@
         <v>0</v>
       </c>
       <c r="N25" t="n">
+        <v>13</v>
+      </c>
+      <c r="O25" t="n">
         <v>6</v>
       </c>
-      <c r="O25" t="n">
+      <c r="P25" t="n">
         <v>5</v>
       </c>
-      <c r="P25" t="n">
+      <c r="Q25" t="n">
         <v>21</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="R25" t="n">
         <v>-2</v>
       </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="S25" t="inlineStr">
         <is>
           <t>@</t>
         </is>
       </c>
       <c r="T25" t="n">
-        <v>-0.7</v>
+        <v>-0.8</v>
       </c>
       <c r="U25" t="n">
-        <v>-3.4</v>
+        <v>-3.3</v>
       </c>
       <c r="V25" t="n">
         <v>5</v>
@@ -4434,12 +4426,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Kyle Kuzma</t>
+          <t>Donovan Mitchell</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -4449,7 +4441,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -4458,28 +4450,28 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>25.2</v>
+        <v>16</v>
       </c>
       <c r="G27" t="n">
-        <v>34.2</v>
+        <v>33.5</v>
       </c>
       <c r="H27" t="n">
-        <v>29.9</v>
+        <v>37.9</v>
       </c>
       <c r="I27" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="J27" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K27" t="n">
         <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
@@ -4487,81 +4479,85 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="P27" t="n">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R27" t="n">
-        <v>19</v>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T27" t="n">
-        <v>-0.8</v>
+        <v>-4.3</v>
       </c>
       <c r="U27" t="n">
-        <v>-3</v>
+        <v>-10.9</v>
       </c>
       <c r="V27" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
+          <t>PHX</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE27" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AF27" t="inlineStr">
+        <is>
           <t>LAL</t>
         </is>
       </c>
-      <c r="Y27" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z27" t="n">
-        <v>36</v>
-      </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE27" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AF27" t="inlineStr">
-        <is>
-          <t>POR</t>
-        </is>
-      </c>
       <c r="AG27" t="inlineStr">
         <is>
           <t>@</t>
@@ -4569,17 +4565,17 @@
       </c>
       <c r="AH27" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AI27" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ27" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AK27" t="inlineStr">
@@ -4589,7 +4585,7 @@
       </c>
       <c r="AL27" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>IND</t>
         </is>
       </c>
     </row>
@@ -4797,10 +4793,10 @@
         <v>35</v>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
@@ -4932,12 +4928,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>RJ Barrett</t>
+          <t>Jerami Grant</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -4950,22 +4946,18 @@
           <t>F</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="G30" t="n">
-        <v>30.3</v>
+        <v>26.3</v>
       </c>
       <c r="H30" t="n">
-        <v>27.4</v>
+        <v>27.7</v>
       </c>
       <c r="I30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J30" t="n">
         <v>1</v>
@@ -4977,7 +4969,7 @@
         <v>1</v>
       </c>
       <c r="M30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N30" t="inlineStr">
         <is>
@@ -5010,14 +5002,10 @@
         </is>
       </c>
       <c r="T30" t="n">
-        <v>-0.3</v>
-      </c>
-      <c r="U30" t="n">
-        <v>-7.5</v>
-      </c>
-      <c r="V30" t="n">
-        <v>6</v>
-      </c>
+        <v>-4.1</v>
+      </c>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
       <c r="W30" t="inlineStr">
         <is>
           <t>@</t>
@@ -5025,16 +5013,16 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="Z30" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="AA30" t="inlineStr">
         <is>
@@ -5063,17 +5051,17 @@
       </c>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH30" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AI30" t="inlineStr">
@@ -5083,175 +5071,15 @@
       </c>
       <c r="AJ30" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AK30" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL30" t="inlineStr">
-        <is>
-          <t>BKN</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>POR</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Jerami Grant</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Out</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="n">
-        <v>21</v>
-      </c>
-      <c r="G31" t="n">
-        <v>26.3</v>
-      </c>
-      <c r="H31" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="I31" t="n">
-        <v>2</v>
-      </c>
-      <c r="J31" t="n">
-        <v>1</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" t="n">
-        <v>1</v>
-      </c>
-      <c r="M31" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="T31" t="n">
-        <v>-4.1</v>
-      </c>
-      <c r="U31" t="inlineStr"/>
-      <c r="V31" t="inlineStr"/>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X31" t="inlineStr">
-        <is>
-          <t>CHA</t>
-        </is>
-      </c>
-      <c r="Y31" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z31" t="n">
-        <v>11</v>
-      </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE31" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AF31" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="AG31" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AH31" t="inlineStr">
-        <is>
-          <t>BOS</t>
-        </is>
-      </c>
-      <c r="AI31" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AJ31" t="inlineStr">
-        <is>
-          <t>NOP</t>
-        </is>
-      </c>
-      <c r="AK31" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AL31" t="inlineStr">
         <is>
           <t>GSW</t>
         </is>

</xml_diff>